<commit_message>
Remove obsolete repeated entries
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_PWR_SNSP_Limit.xlsx
+++ b/SuppXLS/Scen_B_PWR_SNSP_Limit.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21086636-7039-4F2B-AB74-AFE4EDCBE048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB69BC97-A3AE-491A-87B2-7BE6767C9449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -705,6 +705,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -714,7 +715,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{D98056AC-E05F-4C3F-AD8B-5B1524962E09}"/>
@@ -1825,12 +1825,12 @@
       <c r="Z15" s="15"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="18"/>
@@ -1914,11 +1914,11 @@
       <c r="A19" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1946,11 +1946,11 @@
       <c r="A20" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
       <c r="G20" s="24"/>
@@ -2038,11 +2038,11 @@
       <c r="A23" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
@@ -2126,11 +2126,11 @@
       <c r="A26" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -2246,11 +2246,11 @@
       <c r="A30" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
       <c r="G30" s="15"/>
@@ -2278,11 +2278,11 @@
       <c r="A31" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
       <c r="G31" s="15"/>
@@ -5002,24 +5002,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -5032,14 +5032,16 @@
         <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:14">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5047,35 +5049,35 @@
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="M7" t="s">
         <v>90</v>
@@ -5088,23 +5090,23 @@
       <c r="B8" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="F8" t="s">
+      <c r="C8" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="G8" t="s">
         <v>72</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>2018</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>89</v>
       </c>
-      <c r="I8" s="30">
+      <c r="J8" s="30">
         <v>-0.65</v>
       </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30" t="s">
-        <v>96</v>
-      </c>
+      <c r="L8" s="30"/>
       <c r="M8">
         <v>0</v>
       </c>
@@ -5114,776 +5116,748 @@
     </row>
     <row r="9" spans="1:14">
       <c r="B9" s="1"/>
-      <c r="C9" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="E9" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" t="s">
+      <c r="F9" s="1"/>
+      <c r="G9" t="s">
         <v>72</v>
       </c>
-      <c r="G9">
-        <f>G8</f>
+      <c r="H9">
+        <f>H8</f>
         <v>2018</v>
       </c>
-      <c r="J9" s="30">
+      <c r="K9" s="30">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="K9" s="30"/>
       <c r="L9" s="30"/>
+      <c r="N9" s="30"/>
     </row>
     <row r="10" spans="1:14">
       <c r="B10" s="1"/>
-      <c r="C10" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="E10" s="31" t="s">
         <v>99</v>
-      </c>
-      <c r="E10" t="s">
-        <v>72</v>
       </c>
       <c r="F10" t="s">
         <v>72</v>
       </c>
-      <c r="G10">
-        <f>G9</f>
+      <c r="G10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10">
+        <f>H9</f>
         <v>2018</v>
       </c>
-      <c r="K10" s="30">
+      <c r="L10" s="30">
         <v>1</v>
       </c>
-      <c r="L10" s="30"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="D11" s="7"/>
-      <c r="F11" t="str">
-        <f>F8</f>
+      <c r="E11" s="7"/>
+      <c r="G11" t="str">
+        <f>G8</f>
         <v>ELCC</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>2020</v>
       </c>
-      <c r="H11" t="str">
-        <f>H8</f>
+      <c r="I11" t="str">
+        <f>I8</f>
         <v>UP</v>
       </c>
-      <c r="I11" s="30">
+      <c r="J11" s="30">
         <v>-0.65</v>
       </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30" t="str">
-        <f>L8</f>
-        <v>UCN, DAYNITE</v>
-      </c>
+      <c r="L11" s="30"/>
       <c r="M11">
         <f>M8</f>
         <v>0</v>
       </c>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="C12" t="str">
-        <f>C9</f>
-        <v>ELE</v>
-      </c>
       <c r="D12" t="str">
         <f>D9</f>
+        <v>ELE</v>
+      </c>
+      <c r="E12" t="str">
+        <f>E9</f>
         <v>P*OCE*,P*SOL*,P*WIN*</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" t="str">
-        <f t="shared" ref="F12:F37" si="0">F9</f>
+      <c r="F12" s="1"/>
+      <c r="G12" t="str">
+        <f t="shared" ref="G12:G37" si="0">G9</f>
         <v>ELCC</v>
       </c>
-      <c r="G12">
-        <f>G11</f>
+      <c r="H12">
+        <f>H11</f>
         <v>2020</v>
       </c>
-      <c r="J12" s="30">
-        <f>J9</f>
+      <c r="K12" s="30">
+        <f>K9</f>
         <v>1</v>
       </c>
-      <c r="K12" s="30"/>
       <c r="L12" s="30"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="C13" t="str">
-        <f>C10</f>
-        <v>IRE</v>
-      </c>
       <c r="D13" t="str">
         <f>D10</f>
-        <v>IMPELC*</v>
+        <v>IRE</v>
       </c>
       <c r="E13" t="str">
         <f>E10</f>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F13" t="str">
+        <f>F10</f>
         <v>ELCC</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G13">
-        <f>G12</f>
+      <c r="H13">
+        <f>H12</f>
         <v>2020</v>
       </c>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30">
-        <f>K10</f>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30">
+        <f>L10</f>
         <v>1</v>
       </c>
-      <c r="L13" s="30"/>
+      <c r="N13" s="30"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="D14" s="7"/>
-      <c r="F14" t="str">
-        <f>F11</f>
+      <c r="E14" s="7"/>
+      <c r="G14" t="str">
+        <f>G11</f>
         <v>ELCC</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>2021</v>
       </c>
-      <c r="H14" t="str">
-        <f>H11</f>
+      <c r="I14" t="str">
+        <f>I11</f>
         <v>UP</v>
       </c>
-      <c r="I14" s="30">
+      <c r="J14" s="30">
         <v>-0.7</v>
       </c>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30" t="str">
-        <f>L11</f>
-        <v>UCN, DAYNITE</v>
-      </c>
+      <c r="L14" s="30"/>
       <c r="M14">
         <f>M11</f>
         <v>0</v>
       </c>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="C15" t="str">
-        <f>C12</f>
-        <v>ELE</v>
-      </c>
       <c r="D15" t="str">
         <f>D12</f>
+        <v>ELE</v>
+      </c>
+      <c r="E15" t="str">
+        <f>E12</f>
         <v>P*OCE*,P*SOL*,P*WIN*</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" t="str">
+      <c r="F15" s="1"/>
+      <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G15">
-        <f>G14</f>
+      <c r="H15">
+        <f>H14</f>
         <v>2021</v>
       </c>
-      <c r="J15" s="30">
-        <f>J12</f>
+      <c r="K15" s="30">
+        <f>K12</f>
         <v>1</v>
       </c>
-      <c r="K15" s="30"/>
       <c r="L15" s="30"/>
+      <c r="N15" s="30"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="C16" t="str">
-        <f>C13</f>
-        <v>IRE</v>
-      </c>
       <c r="D16" t="str">
         <f>D13</f>
-        <v>IMPELC*</v>
+        <v>IRE</v>
       </c>
       <c r="E16" t="str">
         <f>E13</f>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F16" t="str">
+        <f>F13</f>
         <v>ELCC</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G16">
-        <f>G15</f>
+      <c r="H16">
+        <f>H15</f>
         <v>2021</v>
       </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30">
-        <f>K13</f>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30">
+        <f>L13</f>
         <v>1</v>
       </c>
-      <c r="L16" s="30"/>
-    </row>
-    <row r="17" spans="3:13">
-      <c r="D17" s="7"/>
-      <c r="F17" t="str">
-        <f>F14</f>
+      <c r="N16" s="30"/>
+    </row>
+    <row r="17" spans="4:14">
+      <c r="E17" s="7"/>
+      <c r="G17" t="str">
+        <f>G14</f>
         <v>ELCC</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>2022</v>
       </c>
-      <c r="H17" t="str">
-        <f>H14</f>
+      <c r="I17" t="str">
+        <f>I14</f>
         <v>UP</v>
       </c>
-      <c r="I17" s="30">
+      <c r="J17" s="30">
         <v>-0.75</v>
       </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30" t="str">
-        <f>L14</f>
-        <v>UCN, DAYNITE</v>
-      </c>
+      <c r="L17" s="30"/>
       <c r="M17">
         <f>M14</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:13">
-      <c r="C18" t="str">
-        <f>C15</f>
-        <v>ELE</v>
-      </c>
+      <c r="N17" s="30"/>
+    </row>
+    <row r="18" spans="4:14">
       <c r="D18" t="str">
         <f>D15</f>
+        <v>ELE</v>
+      </c>
+      <c r="E18" t="str">
+        <f>E15</f>
         <v>P*OCE*,P*SOL*,P*WIN*</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" t="str">
+      <c r="F18" s="1"/>
+      <c r="G18" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G18">
-        <f>G17</f>
+      <c r="H18">
+        <f>H17</f>
         <v>2022</v>
       </c>
-      <c r="J18" s="30">
-        <f>J15</f>
+      <c r="K18" s="30">
+        <f>K15</f>
         <v>1</v>
       </c>
-      <c r="K18" s="30"/>
       <c r="L18" s="30"/>
-    </row>
-    <row r="19" spans="3:13">
-      <c r="C19" t="str">
-        <f>C16</f>
-        <v>IRE</v>
-      </c>
+      <c r="N18" s="30"/>
+    </row>
+    <row r="19" spans="4:14">
       <c r="D19" t="str">
         <f>D16</f>
-        <v>IMPELC*</v>
+        <v>IRE</v>
       </c>
       <c r="E19" t="str">
         <f>E16</f>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F19" t="str">
+        <f>F16</f>
         <v>ELCC</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G19">
-        <f>G18</f>
+      <c r="H19">
+        <f>H18</f>
         <v>2022</v>
       </c>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30">
-        <f>K16</f>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30">
+        <f>L16</f>
         <v>1</v>
       </c>
-      <c r="L19" s="30"/>
-    </row>
-    <row r="20" spans="3:13">
-      <c r="D20" s="7"/>
-      <c r="F20" t="str">
-        <f>F17</f>
+      <c r="N19" s="30"/>
+    </row>
+    <row r="20" spans="4:14">
+      <c r="E20" s="7"/>
+      <c r="G20" t="str">
+        <f>G17</f>
         <v>ELCC</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>2024</v>
       </c>
-      <c r="H20" t="str">
-        <f>H17</f>
+      <c r="I20" t="str">
+        <f>I17</f>
         <v>UP</v>
       </c>
-      <c r="I20" s="30">
+      <c r="J20" s="30">
         <v>-0.75</v>
       </c>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30" t="str">
-        <f>L17</f>
-        <v>UCN, DAYNITE</v>
-      </c>
+      <c r="L20" s="30"/>
       <c r="M20">
         <f>M17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:13">
-      <c r="C21" t="str">
-        <f>C18</f>
-        <v>ELE</v>
-      </c>
+      <c r="N20" s="30"/>
+    </row>
+    <row r="21" spans="4:14">
       <c r="D21" t="str">
         <f>D18</f>
+        <v>ELE</v>
+      </c>
+      <c r="E21" t="str">
+        <f>E18</f>
         <v>P*OCE*,P*SOL*,P*WIN*</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" t="str">
+      <c r="F21" s="1"/>
+      <c r="G21" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G21">
-        <f>G20</f>
+      <c r="H21">
+        <f>H20</f>
         <v>2024</v>
       </c>
-      <c r="J21" s="30">
-        <f>J18</f>
+      <c r="K21" s="30">
+        <f>K18</f>
         <v>1</v>
       </c>
-      <c r="K21" s="30"/>
       <c r="L21" s="30"/>
-    </row>
-    <row r="22" spans="3:13">
-      <c r="C22" t="str">
-        <f>C19</f>
-        <v>IRE</v>
-      </c>
+      <c r="N21" s="30"/>
+    </row>
+    <row r="22" spans="4:14">
       <c r="D22" t="str">
         <f>D19</f>
-        <v>IMPELC*</v>
+        <v>IRE</v>
       </c>
       <c r="E22" t="str">
         <f>E19</f>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F22" t="str">
+        <f>F19</f>
         <v>ELCC</v>
       </c>
-      <c r="F22" t="str">
+      <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G22">
-        <f>G21</f>
+      <c r="H22">
+        <f>H21</f>
         <v>2024</v>
       </c>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30">
-        <f>K19</f>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30">
+        <f>L19</f>
         <v>1</v>
       </c>
-      <c r="L22" s="30"/>
-    </row>
-    <row r="23" spans="3:13">
-      <c r="D23" s="7"/>
-      <c r="F23" t="str">
-        <f>F20</f>
+      <c r="N22" s="30"/>
+    </row>
+    <row r="23" spans="4:14">
+      <c r="E23" s="7"/>
+      <c r="G23" t="str">
+        <f>G20</f>
         <v>ELCC</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>2025</v>
       </c>
-      <c r="H23" t="str">
-        <f>H20</f>
+      <c r="I23" t="str">
+        <f>I20</f>
         <v>UP</v>
       </c>
-      <c r="I23" s="30">
+      <c r="J23" s="30">
         <v>-0.85</v>
       </c>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30" t="str">
-        <f>L20</f>
-        <v>UCN, DAYNITE</v>
-      </c>
+      <c r="L23" s="30"/>
       <c r="M23">
         <f>M20</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:13">
-      <c r="C24" t="str">
-        <f>C21</f>
-        <v>ELE</v>
-      </c>
+      <c r="N23" s="30"/>
+    </row>
+    <row r="24" spans="4:14">
       <c r="D24" t="str">
         <f>D21</f>
+        <v>ELE</v>
+      </c>
+      <c r="E24" t="str">
+        <f>E21</f>
         <v>P*OCE*,P*SOL*,P*WIN*</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" t="str">
+      <c r="F24" s="1"/>
+      <c r="G24" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G24">
-        <f>G23</f>
+      <c r="H24">
+        <f>H23</f>
         <v>2025</v>
       </c>
-      <c r="J24" s="30">
-        <f>J21</f>
+      <c r="K24" s="30">
+        <f>K21</f>
         <v>1</v>
       </c>
-      <c r="K24" s="30"/>
       <c r="L24" s="30"/>
-    </row>
-    <row r="25" spans="3:13">
-      <c r="C25" t="str">
-        <f>C22</f>
-        <v>IRE</v>
-      </c>
+      <c r="N24" s="30"/>
+    </row>
+    <row r="25" spans="4:14">
       <c r="D25" t="str">
         <f>D22</f>
-        <v>IMPELC*</v>
+        <v>IRE</v>
       </c>
       <c r="E25" t="str">
         <f>E22</f>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F25" t="str">
+        <f>F22</f>
         <v>ELCC</v>
       </c>
-      <c r="F25" t="str">
+      <c r="G25" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G25">
-        <f>G24</f>
+      <c r="H25">
+        <f>H24</f>
         <v>2025</v>
       </c>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30">
-        <f>K22</f>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30">
+        <f>L22</f>
         <v>1</v>
       </c>
-      <c r="L25" s="30"/>
-    </row>
-    <row r="26" spans="3:13">
-      <c r="D26" s="7"/>
-      <c r="F26" t="str">
-        <f>F23</f>
+      <c r="N25" s="30"/>
+    </row>
+    <row r="26" spans="4:14">
+      <c r="E26" s="7"/>
+      <c r="G26" t="str">
+        <f>G23</f>
         <v>ELCC</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>2029</v>
       </c>
-      <c r="H26" t="str">
-        <f>H23</f>
+      <c r="I26" t="str">
+        <f>I23</f>
         <v>UP</v>
       </c>
-      <c r="I26" s="30">
+      <c r="J26" s="30">
         <v>-0.85</v>
       </c>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30" t="str">
-        <f>L23</f>
-        <v>UCN, DAYNITE</v>
-      </c>
+      <c r="L26" s="30"/>
       <c r="M26">
         <f>M23</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="3:13">
-      <c r="C27" t="str">
-        <f>C24</f>
-        <v>ELE</v>
-      </c>
+      <c r="N26" s="30"/>
+    </row>
+    <row r="27" spans="4:14">
       <c r="D27" t="str">
         <f>D24</f>
+        <v>ELE</v>
+      </c>
+      <c r="E27" t="str">
+        <f>E24</f>
         <v>P*OCE*,P*SOL*,P*WIN*</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="F27" t="str">
+      <c r="F27" s="1"/>
+      <c r="G27" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G27">
-        <f>G26</f>
+      <c r="H27">
+        <f>H26</f>
         <v>2029</v>
       </c>
-      <c r="J27" s="30">
-        <f>J24</f>
+      <c r="K27" s="30">
+        <f>K24</f>
         <v>1</v>
       </c>
-      <c r="K27" s="30"/>
       <c r="L27" s="30"/>
-    </row>
-    <row r="28" spans="3:13">
-      <c r="C28" t="str">
-        <f>C25</f>
-        <v>IRE</v>
-      </c>
+      <c r="N27" s="30"/>
+    </row>
+    <row r="28" spans="4:14">
       <c r="D28" t="str">
         <f>D25</f>
-        <v>IMPELC*</v>
+        <v>IRE</v>
       </c>
       <c r="E28" t="str">
         <f>E25</f>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F28" t="str">
+        <f>F25</f>
         <v>ELCC</v>
       </c>
-      <c r="F28" t="str">
+      <c r="G28" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G28">
-        <f>G27</f>
+      <c r="H28">
+        <f>H27</f>
         <v>2029</v>
       </c>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30">
-        <f>K25</f>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30">
+        <f>L25</f>
         <v>1</v>
       </c>
-      <c r="L28" s="30"/>
-    </row>
-    <row r="29" spans="3:13">
-      <c r="D29" s="7"/>
-      <c r="F29" t="str">
-        <f>F26</f>
+      <c r="N28" s="30"/>
+    </row>
+    <row r="29" spans="4:14">
+      <c r="E29" s="7"/>
+      <c r="G29" t="str">
+        <f>G26</f>
         <v>ELCC</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>2030</v>
       </c>
-      <c r="H29" t="str">
-        <f>H26</f>
+      <c r="I29" t="str">
+        <f>I26</f>
         <v>UP</v>
       </c>
-      <c r="I29" s="30">
+      <c r="J29" s="30">
         <v>-0.95</v>
       </c>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30" t="str">
-        <f>L26</f>
-        <v>UCN, DAYNITE</v>
-      </c>
+      <c r="L29" s="30"/>
       <c r="M29">
         <f>M26</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="3:13">
-      <c r="C30" t="str">
-        <f>C27</f>
-        <v>ELE</v>
-      </c>
+      <c r="N29" s="30"/>
+    </row>
+    <row r="30" spans="4:14">
       <c r="D30" t="str">
         <f>D27</f>
+        <v>ELE</v>
+      </c>
+      <c r="E30" t="str">
+        <f>E27</f>
         <v>P*OCE*,P*SOL*,P*WIN*</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" t="str">
+      <c r="F30" s="1"/>
+      <c r="G30" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G30">
-        <f>G29</f>
+      <c r="H30">
+        <f>H29</f>
         <v>2030</v>
       </c>
-      <c r="J30" s="30">
-        <f>J27</f>
+      <c r="K30" s="30">
+        <f>K27</f>
         <v>1</v>
       </c>
-      <c r="K30" s="30"/>
       <c r="L30" s="30"/>
-    </row>
-    <row r="31" spans="3:13">
-      <c r="C31" t="str">
-        <f>C28</f>
-        <v>IRE</v>
-      </c>
+      <c r="N30" s="30"/>
+    </row>
+    <row r="31" spans="4:14">
       <c r="D31" t="str">
         <f>D28</f>
-        <v>IMPELC*</v>
+        <v>IRE</v>
       </c>
       <c r="E31" t="str">
         <f>E28</f>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F31" t="str">
+        <f>F28</f>
         <v>ELCC</v>
       </c>
-      <c r="F31" t="str">
+      <c r="G31" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G31">
-        <f>G30</f>
+      <c r="H31">
+        <f>H30</f>
         <v>2030</v>
       </c>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30">
-        <f>K28</f>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30">
+        <f>L28</f>
         <v>1</v>
       </c>
-      <c r="L31" s="30"/>
-    </row>
-    <row r="32" spans="3:13">
-      <c r="D32" s="7"/>
-      <c r="F32" t="str">
-        <f>F29</f>
+      <c r="N31" s="30"/>
+    </row>
+    <row r="32" spans="4:14">
+      <c r="E32" s="7"/>
+      <c r="G32" t="str">
+        <f>G29</f>
         <v>ELCC</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>2034</v>
       </c>
-      <c r="H32" t="str">
-        <f>H29</f>
+      <c r="I32" t="str">
+        <f>I29</f>
         <v>UP</v>
       </c>
-      <c r="I32" s="30">
+      <c r="J32" s="30">
         <v>-0.95</v>
       </c>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30" t="str">
-        <f>L29</f>
-        <v>UCN, DAYNITE</v>
-      </c>
+      <c r="L32" s="30"/>
       <c r="M32">
         <f>M29</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="3:13">
-      <c r="C33" t="str">
-        <f>C30</f>
-        <v>ELE</v>
-      </c>
+      <c r="N32" s="30"/>
+    </row>
+    <row r="33" spans="4:14">
       <c r="D33" t="str">
         <f>D30</f>
+        <v>ELE</v>
+      </c>
+      <c r="E33" t="str">
+        <f>E30</f>
         <v>P*OCE*,P*SOL*,P*WIN*</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="F33" t="str">
+      <c r="F33" s="1"/>
+      <c r="G33" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G33">
-        <f>G32</f>
+      <c r="H33">
+        <f>H32</f>
         <v>2034</v>
       </c>
-      <c r="J33" s="30">
-        <f>J30</f>
+      <c r="K33" s="30">
+        <f>K30</f>
         <v>1</v>
       </c>
-      <c r="K33" s="30"/>
       <c r="L33" s="30"/>
-    </row>
-    <row r="34" spans="3:13">
-      <c r="C34" t="str">
-        <f>C31</f>
-        <v>IRE</v>
-      </c>
+      <c r="N33" s="30"/>
+    </row>
+    <row r="34" spans="4:14">
       <c r="D34" t="str">
         <f>D31</f>
-        <v>IMPELC*</v>
+        <v>IRE</v>
       </c>
       <c r="E34" t="str">
         <f>E31</f>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F34" t="str">
+        <f>F31</f>
         <v>ELCC</v>
       </c>
-      <c r="F34" t="str">
+      <c r="G34" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G34">
-        <f>G33</f>
+      <c r="H34">
+        <f>H33</f>
         <v>2034</v>
       </c>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30">
-        <f>K31</f>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30">
+        <f>L31</f>
         <v>1</v>
       </c>
-      <c r="L34" s="30"/>
-    </row>
-    <row r="35" spans="3:13">
-      <c r="D35" s="7"/>
-      <c r="F35" t="str">
-        <f>F32</f>
+      <c r="N34" s="30"/>
+    </row>
+    <row r="35" spans="4:14">
+      <c r="E35" s="7"/>
+      <c r="G35" t="str">
+        <f>G32</f>
         <v>ELCC</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>2035</v>
       </c>
-      <c r="H35" t="str">
-        <f>H32</f>
+      <c r="I35" t="str">
+        <f>I32</f>
         <v>UP</v>
       </c>
-      <c r="I35" s="30">
+      <c r="J35" s="30">
         <v>-1</v>
       </c>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30" t="str">
-        <f>L32</f>
-        <v>UCN, DAYNITE</v>
-      </c>
+      <c r="L35" s="30"/>
       <c r="M35">
         <f>M32</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="3:13">
-      <c r="C36" t="str">
-        <f>C33</f>
-        <v>ELE</v>
-      </c>
+      <c r="N35" s="30"/>
+    </row>
+    <row r="36" spans="4:14">
       <c r="D36" t="str">
         <f>D33</f>
+        <v>ELE</v>
+      </c>
+      <c r="E36" t="str">
+        <f>E33</f>
         <v>P*OCE*,P*SOL*,P*WIN*</v>
       </c>
-      <c r="E36" s="1"/>
-      <c r="F36" t="str">
+      <c r="F36" s="1"/>
+      <c r="G36" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G36">
-        <f>G35</f>
+      <c r="H36">
+        <f>H35</f>
         <v>2035</v>
       </c>
-      <c r="J36" s="30">
-        <f>J33</f>
+      <c r="K36" s="30">
+        <f>K33</f>
         <v>1</v>
       </c>
-      <c r="K36" s="30"/>
       <c r="L36" s="30"/>
-    </row>
-    <row r="37" spans="3:13">
-      <c r="C37" t="str">
-        <f>C34</f>
-        <v>IRE</v>
-      </c>
+      <c r="N36" s="30"/>
+    </row>
+    <row r="37" spans="4:14">
       <c r="D37" t="str">
         <f>D34</f>
-        <v>IMPELC*</v>
+        <v>IRE</v>
       </c>
       <c r="E37" t="str">
         <f>E34</f>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F37" t="str">
+        <f>F34</f>
         <v>ELCC</v>
       </c>
-      <c r="F37" t="str">
+      <c r="G37" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="G37">
-        <f>G36</f>
+      <c r="H37">
+        <f>H36</f>
         <v>2035</v>
       </c>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30">
-        <f>K34</f>
+      <c r="K37" s="30"/>
+      <c r="L37" s="30">
+        <f>L34</f>
         <v>1</v>
       </c>
-      <c r="L37" s="30"/>
-    </row>
-    <row r="38" spans="3:13">
-      <c r="G38">
+      <c r="N37" s="30"/>
+    </row>
+    <row r="38" spans="4:14">
+      <c r="H38">
         <v>0</v>
       </c>
-      <c r="H38" t="str">
-        <f>H35</f>
+      <c r="I38" t="str">
+        <f>I35</f>
         <v>UP</v>
-      </c>
-      <c r="L38" s="30" t="str">
-        <f>L35</f>
-        <v>UCN, DAYNITE</v>
       </c>
       <c r="M38">
         <v>5</v>
       </c>
+      <c r="N38" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Include electricity export in the SNSP limit calculation
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_PWR_SNSP_Limit.xlsx
+++ b/SuppXLS/Scen_B_PWR_SNSP_Limit.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB69BC97-A3AE-491A-87B2-7BE6767C9449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568A904C-D308-4302-B3AB-BD9C1C4F5176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
   <si>
     <t>UC_N</t>
   </si>
@@ -377,6 +377,15 @@
   <si>
     <t>Pset_CO</t>
   </si>
+  <si>
+    <t>EXPELC*</t>
+  </si>
+  <si>
+    <t>UC_IRE-E</t>
+  </si>
+  <si>
+    <t>Pset_CI</t>
+  </si>
 </sst>
 </file>
 
@@ -385,7 +394,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,6 +511,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -634,7 +650,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -715,6 +731,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{D98056AC-E05F-4C3F-AD8B-5B1524962E09}"/>
@@ -5000,52 +5017,56 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:16">
       <c r="B4" s="2" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:16">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:14">
-      <c r="I6" t="s">
+    <row r="6" spans="1:16">
+      <c r="J6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:16">
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
@@ -5061,32 +5082,38 @@
       <c r="F7" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O7" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="P7" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:16">
       <c r="B8" t="s">
         <v>94</v>
       </c>
@@ -5094,27 +5121,28 @@
         <v>96</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>72</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>2018</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="30">
+      <c r="K8" s="30">
         <v>-0.65</v>
       </c>
-      <c r="L8" s="30"/>
-      <c r="M8">
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8">
         <v>0</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="P8" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:16">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" t="s">
@@ -5124,21 +5152,23 @@
         <v>11</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" t="s">
         <v>72</v>
       </c>
-      <c r="H9">
-        <f>H8</f>
+      <c r="I9">
+        <f>I8</f>
         <v>2018</v>
       </c>
-      <c r="K9" s="30">
+      <c r="L9" s="30">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
       <c r="N9" s="30"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="P9" s="30"/>
+    </row>
+    <row r="10" spans="1:16">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
@@ -5150,714 +5180,1037 @@
       <c r="F10" t="s">
         <v>72</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>72</v>
       </c>
-      <c r="H10">
-        <f>H9</f>
+      <c r="I10">
+        <f>I9</f>
         <v>2018</v>
       </c>
-      <c r="L10" s="30">
+      <c r="M10" s="30">
         <v>1</v>
       </c>
       <c r="N10" s="30"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="E11" s="7"/>
-      <c r="G11" t="str">
-        <f>G8</f>
+      <c r="P10" s="30"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11">
+        <v>2018</v>
+      </c>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30">
+        <f>-1-K8</f>
+        <v>-0.35</v>
+      </c>
+      <c r="P11" s="30"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="E12" s="7"/>
+      <c r="H12" t="str">
+        <f t="shared" ref="H12:H44" si="0">H8</f>
         <v>ELCC</v>
       </c>
-      <c r="H11">
+      <c r="I12">
         <v>2020</v>
       </c>
-      <c r="I11" t="str">
-        <f>I8</f>
+      <c r="J12" t="str">
+        <f>J8</f>
         <v>UP</v>
       </c>
-      <c r="J11" s="30">
+      <c r="K12" s="30">
         <v>-0.65</v>
       </c>
-      <c r="L11" s="30"/>
-      <c r="M11">
-        <f>M8</f>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12">
+        <f>O8</f>
         <v>0</v>
       </c>
-      <c r="N11" s="30"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="D12" t="str">
-        <f>D9</f>
+      <c r="P12" s="30"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="D13" t="str">
+        <f t="shared" ref="D13:E15" si="1">D9</f>
         <v>ELE</v>
       </c>
-      <c r="E12" t="str">
-        <f>E9</f>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
         <v>P*OCE*,P*SOL*,P*WIN*</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" t="str">
-        <f t="shared" ref="G12:G37" si="0">G9</f>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H12">
-        <f>H11</f>
+      <c r="I13">
+        <f>I12</f>
         <v>2020</v>
       </c>
-      <c r="K12" s="30">
-        <f>K9</f>
+      <c r="L13" s="30">
+        <f>L9</f>
         <v>1</v>
       </c>
-      <c r="L12" s="30"/>
-      <c r="N12" s="30"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="D13" t="str">
-        <f>D10</f>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="P13" s="30"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
         <v>IRE</v>
       </c>
-      <c r="E13" t="str">
-        <f>E10</f>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
         <v>IMPELC*</v>
       </c>
-      <c r="F13" t="str">
+      <c r="F14" t="str">
         <f>F10</f>
         <v>ELCC</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H13">
-        <f>H12</f>
+      <c r="I14">
+        <f>I13</f>
         <v>2020</v>
       </c>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30">
-        <f>L10</f>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30">
+        <f>M10</f>
         <v>1</v>
       </c>
-      <c r="N13" s="30"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="E14" s="7"/>
-      <c r="G14" t="str">
+      <c r="N14" s="30"/>
+      <c r="P14" s="30"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>IRE</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>EXPELC*</v>
+      </c>
+      <c r="G15" t="str">
         <f>G11</f>
         <v>ELCC</v>
       </c>
-      <c r="H14">
-        <v>2021</v>
-      </c>
-      <c r="I14" t="str">
-        <f>I11</f>
-        <v>UP</v>
-      </c>
-      <c r="J14" s="30">
-        <v>-0.7</v>
-      </c>
-      <c r="L14" s="30"/>
-      <c r="M14">
-        <f>M11</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="30"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="D15" t="str">
-        <f>D12</f>
-        <v>ELE</v>
-      </c>
-      <c r="E15" t="str">
-        <f>E12</f>
-        <v>P*OCE*,P*SOL*,P*WIN*</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" t="str">
+      <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H15">
-        <f>H14</f>
-        <v>2021</v>
-      </c>
-      <c r="K15" s="30">
-        <f>K12</f>
-        <v>1</v>
+      <c r="I15">
+        <f>I14</f>
+        <v>2020</v>
       </c>
       <c r="L15" s="30"/>
-      <c r="N15" s="30"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="D16" t="str">
-        <f>D13</f>
-        <v>IRE</v>
-      </c>
-      <c r="E16" t="str">
-        <f>E13</f>
-        <v>IMPELC*</v>
-      </c>
-      <c r="F16" t="str">
-        <f>F13</f>
-        <v>ELCC</v>
-      </c>
-      <c r="G16" t="str">
+      <c r="M15" s="30"/>
+      <c r="N15" s="30">
+        <f>-1-K12</f>
+        <v>-0.35</v>
+      </c>
+      <c r="P15" s="30"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="E16" s="7"/>
+      <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H16">
-        <f>H15</f>
+      <c r="I16">
         <v>2021</v>
       </c>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30">
+      <c r="J16" t="str">
+        <f>J12</f>
+        <v>UP</v>
+      </c>
+      <c r="K16" s="30">
+        <v>-0.7</v>
+      </c>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16">
+        <f>O12</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="30"/>
+    </row>
+    <row r="17" spans="4:16">
+      <c r="D17" t="str">
+        <f t="shared" ref="D17:E19" si="2">D13</f>
+        <v>ELE</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v>P*OCE*,P*SOL*,P*WIN*</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I17">
+        <f>I16</f>
+        <v>2021</v>
+      </c>
+      <c r="L17" s="30">
         <f>L13</f>
         <v>1</v>
       </c>
-      <c r="N16" s="30"/>
-    </row>
-    <row r="17" spans="4:14">
-      <c r="E17" s="7"/>
-      <c r="G17" t="str">
-        <f>G14</f>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="P17" s="30"/>
+    </row>
+    <row r="18" spans="4:16">
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>IRE</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F18" t="str">
+        <f>F14</f>
         <v>ELCC</v>
       </c>
-      <c r="H17">
-        <v>2022</v>
-      </c>
-      <c r="I17" t="str">
-        <f>I14</f>
-        <v>UP</v>
-      </c>
-      <c r="J17" s="30">
-        <v>-0.75</v>
-      </c>
-      <c r="L17" s="30"/>
-      <c r="M17">
-        <f>M14</f>
-        <v>0</v>
-      </c>
-      <c r="N17" s="30"/>
-    </row>
-    <row r="18" spans="4:14">
-      <c r="D18" t="str">
-        <f>D15</f>
-        <v>ELE</v>
-      </c>
-      <c r="E18" t="str">
-        <f>E15</f>
-        <v>P*OCE*,P*SOL*,P*WIN*</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" t="str">
+      <c r="H18" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H18">
-        <f>H17</f>
-        <v>2022</v>
-      </c>
-      <c r="K18" s="30">
-        <f>K15</f>
+      <c r="I18">
+        <f>I17</f>
+        <v>2021</v>
+      </c>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30">
+        <f>M14</f>
         <v>1</v>
       </c>
-      <c r="L18" s="30"/>
       <c r="N18" s="30"/>
-    </row>
-    <row r="19" spans="4:14">
+      <c r="P18" s="30"/>
+    </row>
+    <row r="19" spans="4:16">
       <c r="D19" t="str">
-        <f>D16</f>
+        <f t="shared" si="2"/>
         <v>IRE</v>
       </c>
       <c r="E19" t="str">
-        <f>E16</f>
-        <v>IMPELC*</v>
-      </c>
-      <c r="F19" t="str">
-        <f>F16</f>
+        <f t="shared" si="2"/>
+        <v>EXPELC*</v>
+      </c>
+      <c r="G19" t="str">
+        <f>G15</f>
         <v>ELCC</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H19">
-        <f>H18</f>
-        <v>2022</v>
-      </c>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30">
-        <f>L16</f>
-        <v>1</v>
-      </c>
-      <c r="N19" s="30"/>
-    </row>
-    <row r="20" spans="4:14">
+      <c r="I19">
+        <f>I18</f>
+        <v>2021</v>
+      </c>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30">
+        <f>-1-K16</f>
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="P19" s="30"/>
+    </row>
+    <row r="20" spans="4:16">
       <c r="E20" s="7"/>
-      <c r="G20" t="str">
-        <f>G17</f>
-        <v>ELCC</v>
-      </c>
-      <c r="H20">
-        <v>2024</v>
-      </c>
-      <c r="I20" t="str">
-        <f>I17</f>
-        <v>UP</v>
-      </c>
-      <c r="J20" s="30">
-        <v>-0.75</v>
-      </c>
-      <c r="L20" s="30"/>
-      <c r="M20">
-        <f>M17</f>
-        <v>0</v>
-      </c>
-      <c r="N20" s="30"/>
-    </row>
-    <row r="21" spans="4:14">
-      <c r="D21" t="str">
-        <f>D18</f>
-        <v>ELE</v>
-      </c>
-      <c r="E21" t="str">
-        <f>E18</f>
-        <v>P*OCE*,P*SOL*,P*WIN*</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" t="str">
+      <c r="H20" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H21">
-        <f>H20</f>
-        <v>2024</v>
-      </c>
-      <c r="K21" s="30">
-        <f>K18</f>
-        <v>1</v>
-      </c>
-      <c r="L21" s="30"/>
-      <c r="N21" s="30"/>
-    </row>
-    <row r="22" spans="4:14">
-      <c r="D22" t="str">
-        <f>D19</f>
-        <v>IRE</v>
-      </c>
-      <c r="E22" t="str">
-        <f>E19</f>
-        <v>IMPELC*</v>
-      </c>
-      <c r="F22" t="str">
-        <f>F19</f>
-        <v>ELCC</v>
-      </c>
-      <c r="G22" t="str">
+      <c r="I20">
+        <v>2022</v>
+      </c>
+      <c r="J20" t="str">
+        <f>J16</f>
+        <v>UP</v>
+      </c>
+      <c r="K20" s="30">
+        <v>-0.75</v>
+      </c>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20">
+        <f>O16</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="30"/>
+    </row>
+    <row r="21" spans="4:16">
+      <c r="D21" t="str">
+        <f t="shared" ref="D21:E23" si="3">D17</f>
+        <v>ELE</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="3"/>
+        <v>P*OCE*,P*SOL*,P*WIN*</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H22">
-        <f>H21</f>
-        <v>2024</v>
-      </c>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30">
-        <f>L19</f>
+      <c r="I21">
+        <f>I20</f>
+        <v>2022</v>
+      </c>
+      <c r="L21" s="30">
+        <f>L17</f>
         <v>1</v>
       </c>
-      <c r="N22" s="30"/>
-    </row>
-    <row r="23" spans="4:14">
-      <c r="E23" s="7"/>
-      <c r="G23" t="str">
-        <f>G20</f>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="P21" s="30"/>
+    </row>
+    <row r="22" spans="4:16">
+      <c r="D22" t="str">
+        <f t="shared" si="3"/>
+        <v>IRE</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="3"/>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F22" t="str">
+        <f>F18</f>
         <v>ELCC</v>
       </c>
-      <c r="H23">
-        <v>2025</v>
-      </c>
-      <c r="I23" t="str">
-        <f>I20</f>
-        <v>UP</v>
-      </c>
-      <c r="J23" s="30">
-        <v>-0.85</v>
-      </c>
-      <c r="L23" s="30"/>
-      <c r="M23">
-        <f>M20</f>
-        <v>0</v>
-      </c>
-      <c r="N23" s="30"/>
-    </row>
-    <row r="24" spans="4:14">
-      <c r="D24" t="str">
-        <f>D21</f>
-        <v>ELE</v>
-      </c>
-      <c r="E24" t="str">
-        <f>E21</f>
-        <v>P*OCE*,P*SOL*,P*WIN*</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="G24" t="str">
+      <c r="H22" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H24">
-        <f>H23</f>
-        <v>2025</v>
+      <c r="I22">
+        <f>I21</f>
+        <v>2022</v>
+      </c>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30">
+        <f>M18</f>
+        <v>1</v>
+      </c>
+      <c r="N22" s="30"/>
+      <c r="P22" s="30"/>
+    </row>
+    <row r="23" spans="4:16">
+      <c r="D23" t="str">
+        <f t="shared" si="3"/>
+        <v>IRE</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="3"/>
+        <v>EXPELC*</v>
+      </c>
+      <c r="G23" t="str">
+        <f>G19</f>
+        <v>ELCC</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I23">
+        <f>I22</f>
+        <v>2022</v>
+      </c>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30">
+        <f>-1-K20</f>
+        <v>-0.25</v>
+      </c>
+      <c r="P23" s="30"/>
+    </row>
+    <row r="24" spans="4:16">
+      <c r="E24" s="7"/>
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I24">
+        <v>2024</v>
+      </c>
+      <c r="J24" t="str">
+        <f>J20</f>
+        <v>UP</v>
       </c>
       <c r="K24" s="30">
-        <f>K21</f>
+        <v>-0.75</v>
+      </c>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24">
+        <f>O20</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="30"/>
+    </row>
+    <row r="25" spans="4:16">
+      <c r="D25" t="str">
+        <f t="shared" ref="D25:E27" si="4">D21</f>
+        <v>ELE</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="4"/>
+        <v>P*OCE*,P*SOL*,P*WIN*</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I25">
+        <f>I24</f>
+        <v>2024</v>
+      </c>
+      <c r="L25" s="30">
+        <f>L21</f>
         <v>1</v>
       </c>
-      <c r="L24" s="30"/>
-      <c r="N24" s="30"/>
-    </row>
-    <row r="25" spans="4:14">
-      <c r="D25" t="str">
-        <f>D22</f>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="P25" s="30"/>
+    </row>
+    <row r="26" spans="4:16">
+      <c r="D26" t="str">
+        <f t="shared" si="4"/>
         <v>IRE</v>
       </c>
-      <c r="E25" t="str">
-        <f>E22</f>
+      <c r="E26" t="str">
+        <f t="shared" si="4"/>
         <v>IMPELC*</v>
       </c>
-      <c r="F25" t="str">
+      <c r="F26" t="str">
         <f>F22</f>
         <v>ELCC</v>
       </c>
-      <c r="G25" t="str">
+      <c r="H26" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H25">
-        <f>H24</f>
-        <v>2025</v>
-      </c>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30">
-        <f>L22</f>
+      <c r="I26">
+        <f>I25</f>
+        <v>2024</v>
+      </c>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30">
+        <f>M22</f>
         <v>1</v>
       </c>
-      <c r="N25" s="30"/>
-    </row>
-    <row r="26" spans="4:14">
-      <c r="E26" s="7"/>
-      <c r="G26" t="str">
+      <c r="N26" s="30"/>
+      <c r="P26" s="30"/>
+    </row>
+    <row r="27" spans="4:16">
+      <c r="D27" t="str">
+        <f t="shared" si="4"/>
+        <v>IRE</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="4"/>
+        <v>EXPELC*</v>
+      </c>
+      <c r="G27" t="str">
         <f>G23</f>
         <v>ELCC</v>
       </c>
-      <c r="H26">
-        <v>2029</v>
-      </c>
-      <c r="I26" t="str">
-        <f>I23</f>
-        <v>UP</v>
-      </c>
-      <c r="J26" s="30">
-        <v>-0.85</v>
-      </c>
-      <c r="L26" s="30"/>
-      <c r="M26">
-        <f>M23</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="30"/>
-    </row>
-    <row r="27" spans="4:14">
-      <c r="D27" t="str">
-        <f>D24</f>
-        <v>ELE</v>
-      </c>
-      <c r="E27" t="str">
-        <f>E24</f>
-        <v>P*OCE*,P*SOL*,P*WIN*</v>
-      </c>
-      <c r="F27" s="1"/>
-      <c r="G27" t="str">
+      <c r="H27" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H27">
-        <f>H26</f>
-        <v>2029</v>
-      </c>
-      <c r="K27" s="30">
-        <f>K24</f>
-        <v>1</v>
+      <c r="I27">
+        <f>I26</f>
+        <v>2024</v>
       </c>
       <c r="L27" s="30"/>
-      <c r="N27" s="30"/>
-    </row>
-    <row r="28" spans="4:14">
-      <c r="D28" t="str">
-        <f>D25</f>
-        <v>IRE</v>
-      </c>
-      <c r="E28" t="str">
-        <f>E25</f>
-        <v>IMPELC*</v>
-      </c>
-      <c r="F28" t="str">
-        <f>F25</f>
-        <v>ELCC</v>
-      </c>
-      <c r="G28" t="str">
+      <c r="M27" s="30"/>
+      <c r="N27" s="30">
+        <f>-1-K24</f>
+        <v>-0.25</v>
+      </c>
+      <c r="P27" s="30"/>
+    </row>
+    <row r="28" spans="4:16">
+      <c r="E28" s="7"/>
+      <c r="H28" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H28">
-        <f>H27</f>
-        <v>2029</v>
-      </c>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30">
+      <c r="I28">
+        <v>2025</v>
+      </c>
+      <c r="J28" t="str">
+        <f>J24</f>
+        <v>UP</v>
+      </c>
+      <c r="K28" s="30">
+        <v>-0.85</v>
+      </c>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28">
+        <f>O24</f>
+        <v>0</v>
+      </c>
+      <c r="P28" s="30"/>
+    </row>
+    <row r="29" spans="4:16">
+      <c r="D29" t="str">
+        <f t="shared" ref="D29:E31" si="5">D25</f>
+        <v>ELE</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="5"/>
+        <v>P*OCE*,P*SOL*,P*WIN*</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I29">
+        <f>I28</f>
+        <v>2025</v>
+      </c>
+      <c r="L29" s="30">
         <f>L25</f>
         <v>1</v>
       </c>
-      <c r="N28" s="30"/>
-    </row>
-    <row r="29" spans="4:14">
-      <c r="E29" s="7"/>
-      <c r="G29" t="str">
-        <f>G26</f>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="P29" s="30"/>
+    </row>
+    <row r="30" spans="4:16">
+      <c r="D30" t="str">
+        <f t="shared" si="5"/>
+        <v>IRE</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="5"/>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F30" t="str">
+        <f>F26</f>
         <v>ELCC</v>
       </c>
-      <c r="H29">
-        <v>2030</v>
-      </c>
-      <c r="I29" t="str">
-        <f>I26</f>
-        <v>UP</v>
-      </c>
-      <c r="J29" s="30">
-        <v>-0.95</v>
-      </c>
-      <c r="L29" s="30"/>
-      <c r="M29">
-        <f>M26</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="30"/>
-    </row>
-    <row r="30" spans="4:14">
-      <c r="D30" t="str">
-        <f>D27</f>
-        <v>ELE</v>
-      </c>
-      <c r="E30" t="str">
-        <f>E27</f>
-        <v>P*OCE*,P*SOL*,P*WIN*</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" t="str">
+      <c r="H30" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H30">
-        <f>H29</f>
-        <v>2030</v>
-      </c>
-      <c r="K30" s="30">
-        <f>K27</f>
+      <c r="I30">
+        <f>I29</f>
+        <v>2025</v>
+      </c>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30">
+        <f>M26</f>
         <v>1</v>
       </c>
-      <c r="L30" s="30"/>
       <c r="N30" s="30"/>
-    </row>
-    <row r="31" spans="4:14">
+      <c r="P30" s="30"/>
+    </row>
+    <row r="31" spans="4:16">
       <c r="D31" t="str">
-        <f>D28</f>
+        <f t="shared" si="5"/>
         <v>IRE</v>
       </c>
       <c r="E31" t="str">
-        <f>E28</f>
-        <v>IMPELC*</v>
-      </c>
-      <c r="F31" t="str">
-        <f>F28</f>
+        <f t="shared" si="5"/>
+        <v>EXPELC*</v>
+      </c>
+      <c r="G31" t="str">
+        <f>G27</f>
         <v>ELCC</v>
       </c>
-      <c r="G31" t="str">
+      <c r="H31" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H31">
-        <f>H30</f>
-        <v>2030</v>
-      </c>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30">
-        <f>L28</f>
-        <v>1</v>
-      </c>
-      <c r="N31" s="30"/>
-    </row>
-    <row r="32" spans="4:14">
+      <c r="I31">
+        <f>I30</f>
+        <v>2025</v>
+      </c>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30">
+        <f>-1-K28</f>
+        <v>-0.15000000000000002</v>
+      </c>
+      <c r="P31" s="30"/>
+    </row>
+    <row r="32" spans="4:16">
       <c r="E32" s="7"/>
-      <c r="G32" t="str">
-        <f>G29</f>
-        <v>ELCC</v>
-      </c>
-      <c r="H32">
-        <v>2034</v>
-      </c>
-      <c r="I32" t="str">
-        <f>I29</f>
-        <v>UP</v>
-      </c>
-      <c r="J32" s="30">
-        <v>-0.95</v>
-      </c>
-      <c r="L32" s="30"/>
-      <c r="M32">
-        <f>M29</f>
-        <v>0</v>
-      </c>
-      <c r="N32" s="30"/>
-    </row>
-    <row r="33" spans="4:14">
-      <c r="D33" t="str">
-        <f>D30</f>
-        <v>ELE</v>
-      </c>
-      <c r="E33" t="str">
-        <f>E30</f>
-        <v>P*OCE*,P*SOL*,P*WIN*</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" t="str">
+      <c r="H32" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H33">
-        <f>H32</f>
-        <v>2034</v>
-      </c>
-      <c r="K33" s="30">
-        <f>K30</f>
-        <v>1</v>
-      </c>
-      <c r="L33" s="30"/>
-      <c r="N33" s="30"/>
-    </row>
-    <row r="34" spans="4:14">
-      <c r="D34" t="str">
-        <f>D31</f>
-        <v>IRE</v>
-      </c>
-      <c r="E34" t="str">
-        <f>E31</f>
-        <v>IMPELC*</v>
-      </c>
-      <c r="F34" t="str">
-        <f>F31</f>
-        <v>ELCC</v>
-      </c>
-      <c r="G34" t="str">
+      <c r="I32">
+        <v>2029</v>
+      </c>
+      <c r="J32" t="str">
+        <f>J28</f>
+        <v>UP</v>
+      </c>
+      <c r="K32" s="30">
+        <v>-0.85</v>
+      </c>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32">
+        <f>O28</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="30"/>
+    </row>
+    <row r="33" spans="4:16">
+      <c r="D33" t="str">
+        <f t="shared" ref="D33:E35" si="6">D29</f>
+        <v>ELE</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="6"/>
+        <v>P*OCE*,P*SOL*,P*WIN*</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H34">
-        <f>H33</f>
-        <v>2034</v>
-      </c>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30">
-        <f>L31</f>
+      <c r="I33">
+        <f>I32</f>
+        <v>2029</v>
+      </c>
+      <c r="L33" s="30">
+        <f>L29</f>
         <v>1</v>
       </c>
-      <c r="N34" s="30"/>
-    </row>
-    <row r="35" spans="4:14">
-      <c r="E35" s="7"/>
-      <c r="G35" t="str">
-        <f>G32</f>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="P33" s="30"/>
+    </row>
+    <row r="34" spans="4:16">
+      <c r="D34" t="str">
+        <f t="shared" si="6"/>
+        <v>IRE</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="6"/>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F34" t="str">
+        <f>F30</f>
         <v>ELCC</v>
       </c>
-      <c r="H35">
-        <v>2035</v>
-      </c>
-      <c r="I35" t="str">
-        <f>I32</f>
-        <v>UP</v>
-      </c>
-      <c r="J35" s="30">
-        <v>-1</v>
-      </c>
-      <c r="L35" s="30"/>
-      <c r="M35">
-        <f>M32</f>
-        <v>0</v>
-      </c>
-      <c r="N35" s="30"/>
-    </row>
-    <row r="36" spans="4:14">
-      <c r="D36" t="str">
-        <f>D33</f>
-        <v>ELE</v>
-      </c>
-      <c r="E36" t="str">
-        <f>E33</f>
-        <v>P*OCE*,P*SOL*,P*WIN*</v>
-      </c>
-      <c r="F36" s="1"/>
-      <c r="G36" t="str">
+      <c r="H34" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H36">
-        <f>H35</f>
-        <v>2035</v>
+      <c r="I34">
+        <f>I33</f>
+        <v>2029</v>
+      </c>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30">
+        <f>M30</f>
+        <v>1</v>
+      </c>
+      <c r="N34" s="30"/>
+      <c r="P34" s="30"/>
+    </row>
+    <row r="35" spans="4:16">
+      <c r="D35" t="str">
+        <f t="shared" si="6"/>
+        <v>IRE</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="6"/>
+        <v>EXPELC*</v>
+      </c>
+      <c r="G35" t="str">
+        <f>G31</f>
+        <v>ELCC</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I35">
+        <f>I34</f>
+        <v>2029</v>
+      </c>
+      <c r="L35" s="30"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30">
+        <f>-1-K32</f>
+        <v>-0.15000000000000002</v>
+      </c>
+      <c r="P35" s="30"/>
+    </row>
+    <row r="36" spans="4:16">
+      <c r="E36" s="7"/>
+      <c r="H36" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I36">
+        <v>2030</v>
+      </c>
+      <c r="J36" t="str">
+        <f>J32</f>
+        <v>UP</v>
       </c>
       <c r="K36" s="30">
-        <f>K33</f>
+        <v>-0.95</v>
+      </c>
+      <c r="M36" s="30"/>
+      <c r="N36" s="30"/>
+      <c r="O36">
+        <f>O32</f>
+        <v>0</v>
+      </c>
+      <c r="P36" s="30"/>
+    </row>
+    <row r="37" spans="4:16">
+      <c r="D37" t="str">
+        <f t="shared" ref="D37:E39" si="7">D33</f>
+        <v>ELE</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="7"/>
+        <v>P*OCE*,P*SOL*,P*WIN*</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I37">
+        <f>I36</f>
+        <v>2030</v>
+      </c>
+      <c r="L37" s="30">
+        <f>L33</f>
         <v>1</v>
       </c>
-      <c r="L36" s="30"/>
-      <c r="N36" s="30"/>
-    </row>
-    <row r="37" spans="4:14">
-      <c r="D37" t="str">
-        <f>D34</f>
+      <c r="M37" s="30"/>
+      <c r="N37" s="30"/>
+      <c r="P37" s="30"/>
+    </row>
+    <row r="38" spans="4:16">
+      <c r="D38" t="str">
+        <f t="shared" si="7"/>
         <v>IRE</v>
       </c>
-      <c r="E37" t="str">
-        <f>E34</f>
+      <c r="E38" t="str">
+        <f t="shared" si="7"/>
         <v>IMPELC*</v>
       </c>
-      <c r="F37" t="str">
+      <c r="F38" t="str">
         <f>F34</f>
         <v>ELCC</v>
       </c>
-      <c r="G37" t="str">
+      <c r="H38" t="str">
         <f t="shared" si="0"/>
         <v>ELCC</v>
       </c>
-      <c r="H37">
-        <f>H36</f>
+      <c r="I38">
+        <f>I37</f>
+        <v>2030</v>
+      </c>
+      <c r="L38" s="30"/>
+      <c r="M38" s="30">
+        <f>M34</f>
+        <v>1</v>
+      </c>
+      <c r="N38" s="30"/>
+      <c r="P38" s="30"/>
+    </row>
+    <row r="39" spans="4:16">
+      <c r="D39" t="str">
+        <f t="shared" si="7"/>
+        <v>IRE</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="7"/>
+        <v>EXPELC*</v>
+      </c>
+      <c r="G39" t="str">
+        <f>G35</f>
+        <v>ELCC</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I39">
+        <f>I38</f>
+        <v>2030</v>
+      </c>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30">
+        <f>-1-K36</f>
+        <v>-5.0000000000000044E-2</v>
+      </c>
+      <c r="P39" s="30"/>
+    </row>
+    <row r="40" spans="4:16">
+      <c r="E40" s="7"/>
+      <c r="H40" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I40">
+        <v>2034</v>
+      </c>
+      <c r="J40" t="str">
+        <f>J36</f>
+        <v>UP</v>
+      </c>
+      <c r="K40" s="30">
+        <v>-0.95</v>
+      </c>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40">
+        <f>O36</f>
+        <v>0</v>
+      </c>
+      <c r="P40" s="30"/>
+    </row>
+    <row r="41" spans="4:16">
+      <c r="D41" t="str">
+        <f t="shared" ref="D41:E43" si="8">D37</f>
+        <v>ELE</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="8"/>
+        <v>P*OCE*,P*SOL*,P*WIN*</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I41">
+        <f>I40</f>
+        <v>2034</v>
+      </c>
+      <c r="L41" s="30">
+        <f>L37</f>
+        <v>1</v>
+      </c>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="P41" s="30"/>
+    </row>
+    <row r="42" spans="4:16">
+      <c r="D42" t="str">
+        <f t="shared" si="8"/>
+        <v>IRE</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="8"/>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F42" t="str">
+        <f>F38</f>
+        <v>ELCC</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I42">
+        <f>I41</f>
+        <v>2034</v>
+      </c>
+      <c r="L42" s="30"/>
+      <c r="M42" s="30">
+        <f>M38</f>
+        <v>1</v>
+      </c>
+      <c r="N42" s="30"/>
+      <c r="P42" s="30"/>
+    </row>
+    <row r="43" spans="4:16">
+      <c r="D43" t="str">
+        <f t="shared" si="8"/>
+        <v>IRE</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="8"/>
+        <v>EXPELC*</v>
+      </c>
+      <c r="G43" t="str">
+        <f>G39</f>
+        <v>ELCC</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I43">
+        <f>I42</f>
+        <v>2034</v>
+      </c>
+      <c r="L43" s="30"/>
+      <c r="M43" s="30"/>
+      <c r="N43" s="30">
+        <f>-1-K40</f>
+        <v>-5.0000000000000044E-2</v>
+      </c>
+      <c r="P43" s="30"/>
+    </row>
+    <row r="44" spans="4:16">
+      <c r="E44" s="7"/>
+      <c r="H44" t="str">
+        <f t="shared" si="0"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I44">
         <v>2035</v>
       </c>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30">
-        <f>L34</f>
+      <c r="J44" t="str">
+        <f>J40</f>
+        <v>UP</v>
+      </c>
+      <c r="K44" s="30">
+        <v>-1</v>
+      </c>
+      <c r="M44" s="30"/>
+      <c r="N44" s="30"/>
+      <c r="O44">
+        <f>O40</f>
+        <v>0</v>
+      </c>
+      <c r="P44" s="30"/>
+    </row>
+    <row r="45" spans="4:16">
+      <c r="D45" t="str">
+        <f t="shared" ref="D45:E47" si="9">D41</f>
+        <v>ELE</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="9"/>
+        <v>P*OCE*,P*SOL*,P*WIN*</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" t="str">
+        <f t="shared" ref="H45:H47" si="10">H41</f>
+        <v>ELCC</v>
+      </c>
+      <c r="I45">
+        <f>I44</f>
+        <v>2035</v>
+      </c>
+      <c r="L45" s="30">
+        <f>L41</f>
         <v>1</v>
       </c>
-      <c r="N37" s="30"/>
-    </row>
-    <row r="38" spans="4:14">
-      <c r="H38">
+      <c r="M45" s="30"/>
+      <c r="N45" s="30"/>
+      <c r="P45" s="30"/>
+    </row>
+    <row r="46" spans="4:16">
+      <c r="D46" t="str">
+        <f t="shared" si="9"/>
+        <v>IRE</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="9"/>
+        <v>IMPELC*</v>
+      </c>
+      <c r="F46" t="str">
+        <f>F42</f>
+        <v>ELCC</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="10"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I46">
+        <f>I45</f>
+        <v>2035</v>
+      </c>
+      <c r="L46" s="30"/>
+      <c r="M46" s="30">
+        <f>M42</f>
+        <v>1</v>
+      </c>
+      <c r="N46" s="30"/>
+      <c r="P46" s="30"/>
+    </row>
+    <row r="47" spans="4:16">
+      <c r="D47" t="str">
+        <f t="shared" si="9"/>
+        <v>IRE</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="9"/>
+        <v>EXPELC*</v>
+      </c>
+      <c r="G47" t="str">
+        <f>G43</f>
+        <v>ELCC</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="10"/>
+        <v>ELCC</v>
+      </c>
+      <c r="I47">
+        <f>I46</f>
+        <v>2035</v>
+      </c>
+      <c r="L47" s="30"/>
+      <c r="M47" s="30"/>
+      <c r="N47" s="30">
+        <f>-1-K44</f>
         <v>0</v>
       </c>
-      <c r="I38" t="str">
-        <f>I35</f>
+      <c r="P47" s="30"/>
+    </row>
+    <row r="48" spans="4:16">
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48" t="str">
+        <f>J44</f>
         <v>UP</v>
       </c>
-      <c r="M38">
+      <c r="O48">
         <v>5</v>
       </c>
-      <c r="N38" s="30"/>
+      <c r="P48" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>